<commit_message>
Add attendance management features and improve recognition settings
- Introduced new sidebar options for "Take Attendance" and "Edit Attendance".
- Enhanced the attendance page with date selection and model selection for facial recognition.
- Updated the attendance processing logic to allow for multiple image uploads and improved user interface for selecting images.
- Added functionality to edit existing attendance records and create new ones.
- Updated the recognition model to default to "Facenet512" for better accuracy.
- Improved the display of recognition statistics, including model name and confidence scores.
- Enhanced error handling and user feedback throughout the attendance management process.
</commit_message>
<xml_diff>
--- a/excel_exports/AWP_ENTC_TYB.xlsx
+++ b/excel_exports/AWP_ENTC_TYB.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,106 @@
           <t>2025-06-22_y</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-22_x.1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-22_y.1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-08</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-09</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-10</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-11</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-12</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-13</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-14</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-15</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-16</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-17</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-18</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-19</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-20</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-21</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-22</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Present</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Attendance %</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -486,6 +586,100 @@
           <t>❌</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="W2" t="n">
+        <v>3</v>
+      </c>
+      <c r="X2" t="n">
+        <v>19</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>15.8</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -512,6 +706,100 @@
         <is>
           <t>✅</t>
         </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="W3" t="n">
+        <v>5</v>
+      </c>
+      <c r="X3" t="n">
+        <v>19</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>26.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance attendance processing and reporting features
- Added functionality to process multiple images for attendance in a single run, improving user experience.
- Implemented a reset mechanism for form fields and uploaded files on the "Take Attendance" page.
- Enhanced attendance summary display with detailed metrics and visualizations for recognized students.
- Improved error handling and logging for attendance processing and statistics generation.
- Updated database utility functions for better clarity and performance in attendance reporting.
</commit_message>
<xml_diff>
--- a/excel_exports/AWP_ENTC_TYB.xlsx
+++ b/excel_exports/AWP_ENTC_TYB.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,7 +541,7 @@
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>2025-06-22</t>
+          <t>2025-06-22_x</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
@@ -557,6 +557,11 @@
       <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Attendance %</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-22_y</t>
         </is>
       </c>
     </row>
@@ -680,6 +685,11 @@
       <c r="Y2" t="n">
         <v>15.8</v>
       </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -800,6 +810,55 @@
       </c>
       <c r="Y3" t="n">
         <v>26.3</v>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>EC3268</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Sachin Lonkar</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>sachinlonkar@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor attendance processing and enhance Excel export functionality
- Removed the "Student-wise Reports" button from the sidebar for a cleaner interface.
- Improved Excel export logic by implementing context managers for file handling, ensuring files are properly closed.
- Enhanced error handling during Excel file operations, including logging and user feedback for failures.
- Streamlined attendance marking process with automatic attendance marking and improved user notifications.
- Updated the display of recognized students with a more flexible layout and added visual representation of student photos.
</commit_message>
<xml_diff>
--- a/excel_exports/AWP_ENTC_TYB.xlsx
+++ b/excel_exports/AWP_ENTC_TYB.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,7 +541,7 @@
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>2025-06-22_x</t>
+          <t>2025-06-22_x.2</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
@@ -561,7 +561,17 @@
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>2025-06-22_y</t>
+          <t>2025-06-22_y.2</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-23</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>2025-06-22</t>
         </is>
       </c>
     </row>
@@ -677,15 +687,25 @@
         </is>
       </c>
       <c r="W2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X2" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="Y2" t="n">
-        <v>15.8</v>
+        <v>22.7</v>
       </c>
       <c r="Z2" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
@@ -803,15 +823,25 @@
         </is>
       </c>
       <c r="W3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="X3" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="Y3" t="n">
-        <v>26.3</v>
+        <v>31.8</v>
       </c>
       <c r="Z3" t="inlineStr">
+        <is>
+          <t>✅</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
         <is>
           <t>✅</t>
         </is>
@@ -852,10 +882,138 @@
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
       <c r="Z4" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>EC3213</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Atharva Pabalkar</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>atharvapabalkar@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>EC3221</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Devashish Patil</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>devashishpatil@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>❌</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
         <is>
           <t>❌</t>
         </is>

</xml_diff>